<commit_message>
SUDO CODE FOR PARSING
</commit_message>
<xml_diff>
--- a/heroData.xlsx
+++ b/heroData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlam17\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Users\Alex\Desktop\Android Git\DPSProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -471,16 +471,16 @@
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.75" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="12.875" customWidth="1"/>
+    <col min="4" max="4" width="11.75" customWidth="1"/>
+    <col min="5" max="5" width="10.375" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -525,22 +525,22 @@
         <v>32</v>
       </c>
       <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>36</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>33</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>38</v>
-      </c>
-      <c r="R1" t="s">
-        <v>39</v>
-      </c>
-      <c r="S1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -583,8 +583,8 @@
       <c r="M2">
         <v>1</v>
       </c>
-      <c r="N2" s="1">
-        <v>0</v>
+      <c r="N2">
+        <v>200</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -592,8 +592,8 @@
       <c r="P2">
         <v>0</v>
       </c>
-      <c r="Q2">
-        <v>200</v>
+      <c r="Q2" s="1">
+        <v>0</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -643,7 +643,7 @@
         <v>1</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -652,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -711,7 +711,7 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -762,7 +762,7 @@
         <v>3</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -771,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -821,7 +821,7 @@
         <v>10</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -830,7 +830,7 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -880,7 +880,7 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -889,7 +889,7 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -939,7 +939,7 @@
         <v>1</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -948,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="R8">
         <v>0</v>
@@ -998,22 +998,22 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="N9">
+        <v>200</v>
+      </c>
+      <c r="O9">
+        <v>100</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
         <v>15</v>
       </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="P9">
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
         <v>35</v>
-      </c>
-      <c r="Q9">
-        <v>200</v>
-      </c>
-      <c r="R9">
-        <v>100</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1057,7 +1057,7 @@
         <v>1</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -1066,7 +1066,7 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="R10">
         <v>0</v>
@@ -1116,7 +1116,7 @@
         <v>1</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -1125,7 +1125,7 @@
         <v>0</v>
       </c>
       <c r="Q11">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="R11">
         <v>0</v>
@@ -1176,7 +1176,7 @@
         <v>1.5</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -1185,7 +1185,7 @@
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="R12">
         <v>0</v>
@@ -1235,22 +1235,22 @@
         <v>9</v>
       </c>
       <c r="N13">
+        <v>200</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
         <v>75</v>
       </c>
-      <c r="O13">
-        <v>1</v>
-      </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
-      <c r="Q13">
-        <v>200</v>
-      </c>
       <c r="R13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1294,22 +1294,22 @@
         <v>0</v>
       </c>
       <c r="N14">
+        <v>200</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
         <v>120</v>
       </c>
-      <c r="O14">
-        <v>1</v>
-      </c>
-      <c r="P14">
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14">
         <v>0.9</v>
-      </c>
-      <c r="Q14">
-        <v>200</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-      <c r="S14">
-        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1353,22 +1353,22 @@
         <v>1</v>
       </c>
       <c r="N15">
+        <v>100</v>
+      </c>
+      <c r="O15">
+        <v>400</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
         <v>14</v>
       </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="P15">
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
         <v>7</v>
-      </c>
-      <c r="Q15">
-        <v>100</v>
-      </c>
-      <c r="R15">
-        <v>400</v>
-      </c>
-      <c r="S15">
-        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1412,19 +1412,19 @@
         <v>1</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="P16">
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="S16">
         <v>0</v>
@@ -1472,7 +1472,7 @@
         <v>6</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1481,7 +1481,7 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="R17">
         <v>0</v>
@@ -1531,19 +1531,19 @@
         <v>1.8</v>
       </c>
       <c r="N18">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="O18">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P18">
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="R18">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="S18">
         <v>0</v>
@@ -1589,13 +1589,13 @@
       <c r="M19">
         <v>4</v>
       </c>
-      <c r="Q19">
+      <c r="N19">
         <v>200</v>
       </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
-      <c r="S19">
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
         <v>200</v>
       </c>
     </row>
@@ -1640,22 +1640,22 @@
         <v>0</v>
       </c>
       <c r="N20">
+        <v>200</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
         <v>80</v>
       </c>
-      <c r="O20">
-        <v>1</v>
-      </c>
-      <c r="P20">
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
         <v>1.2</v>
-      </c>
-      <c r="Q20">
-        <v>200</v>
-      </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -1699,7 +1699,7 @@
         <v>0</v>
       </c>
       <c r="N21">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -1708,7 +1708,7 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="R21">
         <v>0</v>
@@ -1758,22 +1758,22 @@
         <v>0</v>
       </c>
       <c r="N22">
+        <v>200</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
         <v>20</v>
       </c>
-      <c r="O22">
-        <v>1</v>
-      </c>
-      <c r="P22">
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
         <v>5</v>
-      </c>
-      <c r="Q22">
-        <v>200</v>
-      </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -1818,22 +1818,22 @@
         <v>0</v>
       </c>
       <c r="N23">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O23">
         <v>0</v>
       </c>
       <c r="P23">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q23">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="R23">
         <v>0</v>
       </c>
       <c r="S23">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -1877,22 +1877,22 @@
         <v>0</v>
       </c>
       <c r="N24">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O24">
         <v>0</v>
       </c>
       <c r="P24">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="Q24">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="R24">
         <v>0</v>
       </c>
       <c r="S24">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>